<commit_message>
add tv-8, add tasks get pressure, get min temperature
</commit_message>
<xml_diff>
--- a/app/celery/tasks/tag/files/tags.xlsx
+++ b/app/celery/tasks/tag/files/tags.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\pyramid\app\celery\tasks\building\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\projects\pyramid\pyramid\app\celery\tasks\tag\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03B5648-C7B8-44B3-9C3F-15D5DD7316D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B71192A-D489-4445-B1D2-BD3388BECFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51690" yWindow="1995" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>title</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Энергия А+ за сутки</t>
+  </si>
+  <si>
+    <t>AverageAbsolutePressurePerDay</t>
+  </si>
+  <si>
+    <t>TemperatureMinPerDay</t>
+  </si>
+  <si>
+    <t>VolumeMaxPerDay</t>
+  </si>
+  <si>
+    <t>Максимальный объем за сутки</t>
+  </si>
+  <si>
+    <t>Минимальная температура за сутки</t>
+  </si>
+  <si>
+    <t>Среднее абсолютное давление за сутки</t>
+  </si>
+  <si>
+    <t>VolumeForwardFixDay</t>
+  </si>
+  <si>
+    <t>Объем в прямом направлении на начало суток</t>
   </si>
 </sst>
 </file>
@@ -398,16 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -467,7 +491,40 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
add tags power task
</commit_message>
<xml_diff>
--- a/app/celery/tasks/tag/files/tags.xlsx
+++ b/app/celery/tasks/tag/files/tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\projects\pyramid\pyramid\app\celery\tasks\tag\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D675B37B-C680-41EC-9AE2-FF4982A990AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1922C77E-159A-4AF2-B3A6-A79FFF73EF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52200" yWindow="2505" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52710" yWindow="3015" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>title</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Объем в прямом направлении на начало суток</t>
+  </si>
+  <si>
+    <t>Мощность</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,8 +526,12 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>